<commit_message>
Correzione TraceId test #6 e #147
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INTERSYSTEMS/InterSystems_Italia_S.r.l/TrakCare/ITXX/report-checklist.xlsx
+++ b/GATEWAY/A1#111INTERSYSTEMS/InterSystems_Italia_S.r.l/TrakCare/ITXX/report-checklist.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmonti\Documents\FSE2.0\it-fse-accreditamento\GATEWAY\A1#111INTERSYSTEMS\InterSystems_Italia_S.r.l\TrakCare\ITXX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BD88F2-2C8A-4912-824B-0FE6BD722D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65789CFF-92E5-4B55-9B00-8D0CDDDBE387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$7:$T$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$7:$T$110</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1557,9 +1557,6 @@
     <t>2023-04-19T10:21:57Z</t>
   </si>
   <si>
-    <t>eae8d69bef653d12</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.10909.4.4.3.f809870a2f31dbfc9fc9863156cd43458bcd6e663ffabe70190fb7ed28705429.d66be3ffe9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -1575,10 +1572,13 @@
     <t>2023-04-19T16:44:56Z</t>
   </si>
   <si>
-    <t>641ec7d64dc680c2</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.50502.4.4.5.b3bcda7f4a4560a4f745597d021ea0a8a39109ad68baa81e07f6ff0961a2fddb.6e9db4190d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d6ba896e12aecce9</t>
+  </si>
+  <si>
+    <t>ae72ee4beb45bf2f</t>
   </si>
 </sst>
 </file>
@@ -2207,7 +2207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" ySplit="7" topLeftCell="E87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
@@ -2360,10 +2360,10 @@
         <v>403</v>
       </c>
       <c r="H8" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>404</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>405</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>24</v>
@@ -2673,13 +2673,13 @@
         <v>45036</v>
       </c>
       <c r="G16" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="8" t="s">
         <v>407</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>408</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>24</v>
@@ -6127,13 +6127,13 @@
         <v>45035</v>
       </c>
       <c r="G88" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="I88" s="8" t="s">
         <v>409</v>
-      </c>
-      <c r="H88" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="I88" s="8" t="s">
-        <v>411</v>
       </c>
       <c r="J88" s="9" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Chiarimenti per i casi con ID [45, 47, 48, 51]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INTERSYSTEMS/InterSystems_Italia_S.r.l/TrakCare/ITXX/report-checklist.xlsx
+++ b/GATEWAY/A1#111INTERSYSTEMS/InterSystems_Italia_S.r.l/TrakCare/ITXX/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmonti\Documents\FSE2.0\it-fse-accreditamento\GATEWAY\A1#111INTERSYSTEMS\InterSystems_Italia_S.r.l\TrakCare\ITXX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65789CFF-92E5-4B55-9B00-8D0CDDDBE387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B89E92-873D-4375-955D-590FFAEF786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="413">
   <si>
     <t>ID</t>
   </si>
@@ -1579,6 +1579,10 @@
   </si>
   <si>
     <t>ae72ee4beb45bf2f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E' facoltà della singola azienda, secondo le proprie policy, configurare il sistema in modo che, in caso di timeout, comunichi o meno la situazione  all'operatore e, nel caso, se il timeout debba essere considerato bloccante o meno.
+Nel caso in cui l'azienda decidesse di far comunque procedere l'operatore per non impattare sull'operatività, il sistema proverà automaticamente a reinviare il documento per la validazione dopo un numero di minuti configurabile, per un numero di volte anch'esso configurabile. </t>
   </si>
 </sst>
 </file>
@@ -2208,10 +2212,10 @@
   <dimension ref="A1:T110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="E87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="L32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,7 +3247,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>45</v>
       </c>
@@ -3272,7 +3276,7 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="Q28" s="9"/>
       <c r="R28" s="10" t="s">
@@ -3312,7 +3316,7 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="Q29" s="9"/>
       <c r="R29" s="10" t="s">
@@ -3352,7 +3356,7 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="Q30" s="9"/>
       <c r="R30" s="10" t="s">
@@ -3363,7 +3367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>51</v>
       </c>
@@ -3392,7 +3396,7 @@
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="Q31" s="9"/>
       <c r="R31" s="10" t="s">

</xml_diff>